<commit_message>
Reduce Page Loading Time from  5 to 6 sec to 500ms
</commit_message>
<xml_diff>
--- a/src/querryRunner/Brands/brands.xlsx
+++ b/src/querryRunner/Brands/brands.xlsx
@@ -1,20 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29127"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006999F4-FE85-4346-8741-A95C8818E165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="7260" yWindow="2124" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
   <si>
     <t>brandName</t>
   </si>
@@ -22,6 +28,36 @@
     <t>category</t>
   </si>
   <si>
+    <t>brand_001</t>
+  </si>
+  <si>
+    <t>brand_002</t>
+  </si>
+  <si>
+    <t>brand_003</t>
+  </si>
+  <si>
+    <t>brand_004</t>
+  </si>
+  <si>
+    <t>brand_005</t>
+  </si>
+  <si>
+    <t>brand_006</t>
+  </si>
+  <si>
+    <t>brand_007</t>
+  </si>
+  <si>
+    <t>brand_008</t>
+  </si>
+  <si>
+    <t>brand_009</t>
+  </si>
+  <si>
+    <t>brand_010</t>
+  </si>
+  <si>
     <t>Apple</t>
   </si>
   <si>
@@ -49,20 +85,23 @@
     <t>HP</t>
   </si>
   <si>
-    <t>Lenovo</t>
-  </si>
-  <si>
     <t>Mobile</t>
   </si>
   <si>
     <t>Computers</t>
+  </si>
+  <si>
+    <t>Brand_id</t>
+  </si>
+  <si>
+    <t>Havells</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +164,21 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -169,7 +216,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -203,6 +250,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -237,9 +285,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -412,99 +461,139 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" customWidth="1"/>
+    <col min="3" max="3" width="31.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>2</v>
       </c>
       <c r="B2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:2">
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>17</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>24</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add POSM Available feature to visit system
- Replace displayChecked with POSMchecked field in database schema
- Add POSM Available radio buttons (Yes/No) to executive visit form
- Update all APIs to handle POSMchecked field properly
- Add POSM Available field to admin visit details modal
- Enhance notification system with visit plan metadata display
- Update executive and admin interfaces for better UX
- Maintain backward compatibility for existing visit data
</commit_message>
<xml_diff>
--- a/src/querryRunner/Brands/brands.xlsx
+++ b/src/querryRunner/Brands/brands.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (2)\Zopper\src\querryRunner\Brands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{006999F4-FE85-4346-8741-A95C8818E165}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C559A05-1D21-411A-97EC-20B2D426F946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7260" yWindow="2124" windowWidth="17280" windowHeight="10500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>brandName</t>
   </si>
@@ -34,67 +34,22 @@
     <t>brand_002</t>
   </si>
   <si>
-    <t>brand_003</t>
-  </si>
-  <si>
-    <t>brand_004</t>
-  </si>
-  <si>
-    <t>brand_005</t>
-  </si>
-  <si>
-    <t>brand_006</t>
-  </si>
-  <si>
-    <t>brand_007</t>
-  </si>
-  <si>
-    <t>brand_008</t>
-  </si>
-  <si>
-    <t>brand_009</t>
-  </si>
-  <si>
     <t>brand_010</t>
   </si>
   <si>
-    <t>Apple</t>
-  </si>
-  <si>
     <t>Samsung</t>
   </si>
   <si>
-    <t>Xiaomi</t>
-  </si>
-  <si>
-    <t>OnePlus</t>
-  </si>
-  <si>
-    <t>Oppo</t>
-  </si>
-  <si>
-    <t>Vivo</t>
-  </si>
-  <si>
-    <t>Motorola</t>
-  </si>
-  <si>
-    <t>Dell</t>
-  </si>
-  <si>
-    <t>HP</t>
-  </si>
-  <si>
-    <t>Mobile</t>
-  </si>
-  <si>
-    <t>Computers</t>
-  </si>
-  <si>
     <t>Brand_id</t>
   </si>
   <si>
     <t>Havells</t>
+  </si>
+  <si>
+    <t>Electronics</t>
+  </si>
+  <si>
+    <t>Godrej</t>
   </si>
 </sst>
 </file>
@@ -462,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,7 +432,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>23</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -491,10 +446,10 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
@@ -502,10 +457,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
@@ -513,87 +468,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
         <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added sales page data in amdina dn exective both
</commit_message>
<xml_diff>
--- a/src/querryRunner/Brands/brands.xlsx
+++ b/src/querryRunner/Brands/brands.xlsx
@@ -5,22 +5,23 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (2)\Zopper\src\querryRunner\Brands\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\visha\Desktop\New folder (4)\Zopper\src\querryRunner\Brands\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C559A05-1D21-411A-97EC-20B2D426F946}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F8DDFE0-6D79-4A27-B8B4-3B9C03E33DBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14616" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="31">
   <si>
     <t>brandName</t>
   </si>
@@ -50,13 +51,76 @@
   </si>
   <si>
     <t>Godrej</t>
+  </si>
+  <si>
+    <t>Category_id</t>
+  </si>
+  <si>
+    <t>categoryName</t>
+  </si>
+  <si>
+    <t>brandIds</t>
+  </si>
+  <si>
+    <t>cat_001</t>
+  </si>
+  <si>
+    <t>AC</t>
+  </si>
+  <si>
+    <t>brand_001,brand_010</t>
+  </si>
+  <si>
+    <t>Godrej, Havells</t>
+  </si>
+  <si>
+    <t>cat_002</t>
+  </si>
+  <si>
+    <t>Laptop</t>
+  </si>
+  <si>
+    <t>cat_003</t>
+  </si>
+  <si>
+    <t>Others</t>
+  </si>
+  <si>
+    <t>cat_004</t>
+  </si>
+  <si>
+    <t>Refrigerator</t>
+  </si>
+  <si>
+    <t>cat_005</t>
+  </si>
+  <si>
+    <t>SmartWatch</t>
+  </si>
+  <si>
+    <t>cat_006</t>
+  </si>
+  <si>
+    <t>Smartphone</t>
+  </si>
+  <si>
+    <t>cat_007</t>
+  </si>
+  <si>
+    <t>Tab</t>
+  </si>
+  <si>
+    <t>cat_008</t>
+  </si>
+  <si>
+    <t>Washing Machine</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -72,16 +136,35 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -104,14 +187,35 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFDDDDDD"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFDDDDDD"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFDDDDDD"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFDDDDDD"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -419,9 +523,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="127" zoomScaleNormal="127" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
-    </sheetView>
+    <sheetView zoomScale="127" zoomScaleNormal="127" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -477,4 +579,151 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9193F39-3E66-4307-9CA1-54D7CEF6978E}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="19.109375" customWidth="1"/>
+    <col min="2" max="2" width="15.5546875" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="28.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="42" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>